<commit_message>
Big and Small - Slimes 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Big and Small - Slimes - 3027202907/Big and Small - Slimes - 3027202907.xlsx
+++ b/Data/Big and Small - Slimes - 3027202907/Big and Small - Slimes - 3027202907.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Big and Small - Slimes - 3027202907\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Big and Small - Slimes - 3027202907\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B016BFA7-A224-4C01-A9D8-43F8BF2BE3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBD200D-6520-4E5E-B4A2-725ABA120F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="4485" windowWidth="28710" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="1278">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3813,6 +3813,50 @@
   </si>
   <si>
     <t>AlienRace.ThingDef_AlienRace+BS_Slime.label</t>
+  </si>
+  <si>
+    <t>BS_SlimeEngulf_New.label</t>
+  </si>
+  <si>
+    <t>BS_SlimeEngulf_New.description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS_SlimeEngulf_New.verbProperties.label</t>
+  </si>
+  <si>
+    <t>BS_SlimeEngulfElixir_New.label</t>
+  </si>
+  <si>
+    <t>BS_SlimeEngulfElixir_New.description</t>
+  </si>
+  <si>
+    <t>BS_SlimeEngulfElixir_New.verbProperties.label</t>
+  </si>
+  <si>
+    <t>engulf</t>
+  </si>
+  <si>
+    <t>Jump at and engulf a target smaller than yourself.</t>
+  </si>
+  <si>
+    <t>Uh-oh</t>
+  </si>
+  <si>
+    <t>elixir engulf</t>
+  </si>
+  <si>
+    <t>Engulf a target smaller than yourself to heal their injuries. Hostile targets will attack back to get free.</t>
+  </si>
+  <si>
+    <t>The ambulance is here!</t>
+  </si>
+  <si>
+    <t>이런..</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구급차가 왔어요!</t>
   </si>
 </sst>
 </file>
@@ -4164,15 +4208,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F429"/>
+  <dimension ref="A1:F436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
-      <selection activeCell="G429" sqref="G429"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D438" sqref="D438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
@@ -10343,6 +10388,90 @@
       </c>
       <c r="F429" s="1" t="s">
         <v>1063</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B431" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B432" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E432" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="433" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B433" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F433" s="1" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="434" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B434" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E434" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F434" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="435" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B435" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E435" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F435" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="436" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B436" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E436" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F436" s="1" t="s">
+        <v>1277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>